<commit_message>
simplify sku save and add anothor save function
</commit_message>
<xml_diff>
--- a/data/上架模板.xlsx
+++ b/data/上架模板.xlsx
@@ -3189,15 +3189,16 @@
   <dimension ref="A1:P1615"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A975" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P17" activeCellId="0" sqref="P17:Q17"/>
+      <selection pane="bottomLeft" activeCell="A990" activeCellId="0" sqref="A990"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="17.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="5" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.81"/>

</xml_diff>